<commit_message>
Added architecture, colorsplash, community_member and wildlife hubs
</commit_message>
<xml_diff>
--- a/Script Templates/All Hubs.xlsx
+++ b/Script Templates/All Hubs.xlsx
@@ -70,10 +70,10 @@
     <t>allwhite</t>
   </si>
   <si>
+    <t>architecture</t>
+  </si>
+  <si>
     <t xml:space="preserve">[ ] </t>
-  </si>
-  <si>
-    <t>architecture</t>
   </si>
   <si>
     <t>artgallery</t>
@@ -1779,20 +1779,28 @@
     </row>
     <row r="12" ht="21.5" customHeight="1">
       <c r="A12" t="s" s="10">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s" s="11">
         <v>19</v>
       </c>
-      <c r="B12" t="s" s="11">
-        <v>20</v>
-      </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
+      <c r="C12" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s" s="11">
+        <v>10</v>
+      </c>
       <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
+      <c r="G12" t="s" s="11">
+        <v>10</v>
+      </c>
     </row>
     <row r="13" ht="21.5" customHeight="1">
       <c r="A13" t="s" s="10">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s" s="11">
         <v>21</v>
@@ -1805,7 +1813,7 @@
     </row>
     <row r="14" ht="21.5" customHeight="1">
       <c r="A14" t="s" s="10">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s" s="11">
         <v>22</v>
@@ -1818,7 +1826,7 @@
     </row>
     <row r="15" ht="21.5" customHeight="1">
       <c r="A15" t="s" s="10">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s" s="11">
         <v>23</v>
@@ -1869,7 +1877,7 @@
     </row>
     <row r="18" ht="21.5" customHeight="1">
       <c r="A18" t="s" s="10">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B18" t="s" s="11">
         <v>26</v>
@@ -1882,16 +1890,24 @@
     </row>
     <row r="19" ht="21.5" customHeight="1">
       <c r="A19" t="s" s="10">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="B19" t="s" s="11">
         <v>27</v>
       </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
+      <c r="C19" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="E19" t="s" s="11">
+        <v>10</v>
+      </c>
       <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
+      <c r="G19" t="s" s="11">
+        <v>10</v>
+      </c>
     </row>
     <row r="20" ht="21.5" customHeight="1">
       <c r="A20" t="s" s="10">
@@ -1914,7 +1930,7 @@
     </row>
     <row r="21" ht="21.5" customHeight="1">
       <c r="A21" t="s" s="10">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s" s="11">
         <v>29</v>
@@ -1927,7 +1943,7 @@
     </row>
     <row r="22" ht="21.5" customHeight="1">
       <c r="A22" t="s" s="10">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s" s="11">
         <v>30</v>
@@ -1959,7 +1975,7 @@
     </row>
     <row r="24" ht="21.5" customHeight="1">
       <c r="A24" t="s" s="10">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B24" t="s" s="11">
         <v>32</v>
@@ -1972,7 +1988,7 @@
     </row>
     <row r="25" ht="21.5" customHeight="1">
       <c r="A25" t="s" s="10">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B25" t="s" s="11">
         <v>33</v>
@@ -2006,7 +2022,7 @@
     </row>
     <row r="27" ht="21.5" customHeight="1">
       <c r="A27" t="s" s="10">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B27" t="s" s="11">
         <v>35</v>
@@ -2038,7 +2054,7 @@
     </row>
     <row r="29" ht="21.5" customHeight="1">
       <c r="A29" t="s" s="10">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B29" t="s" s="11">
         <v>37</v>
@@ -2051,20 +2067,28 @@
     </row>
     <row r="30" ht="21.5" customHeight="1">
       <c r="A30" t="s" s="10">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B30" t="s" s="11">
         <v>38</v>
       </c>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
+      <c r="C30" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="D30" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="E30" t="s" s="11">
+        <v>10</v>
+      </c>
       <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
+      <c r="G30" t="s" s="11">
+        <v>10</v>
+      </c>
     </row>
     <row r="31" ht="21.5" customHeight="1">
       <c r="A31" t="s" s="10">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B31" t="s" s="11">
         <v>39</v>
@@ -2077,7 +2101,7 @@
     </row>
     <row r="32" ht="21.5" customHeight="1">
       <c r="A32" t="s" s="10">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B32" t="s" s="11">
         <v>40</v>
@@ -2090,20 +2114,26 @@
     </row>
     <row r="33" ht="21.5" customHeight="1">
       <c r="A33" t="s" s="10">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="B33" t="s" s="11">
         <v>41</v>
       </c>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
+      <c r="C33" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="D33" t="s" s="11">
+        <v>10</v>
+      </c>
       <c r="E33" s="12"/>
       <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
+      <c r="G33" t="s" s="11">
+        <v>10</v>
+      </c>
     </row>
     <row r="34" ht="21.5" customHeight="1">
       <c r="A34" t="s" s="10">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B34" t="s" s="11">
         <v>42</v>
@@ -2137,7 +2167,7 @@
     </row>
     <row r="36" ht="21.5" customHeight="1">
       <c r="A36" t="s" s="10">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B36" t="s" s="11">
         <v>44</v>
@@ -2150,7 +2180,7 @@
     </row>
     <row r="37" ht="21.5" customHeight="1">
       <c r="A37" t="s" s="10">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B37" t="s" s="11">
         <v>45</v>
@@ -2220,7 +2250,7 @@
     </row>
     <row r="41" ht="21.5" customHeight="1">
       <c r="A41" t="s" s="10">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B41" t="s" s="11">
         <v>49</v>
@@ -2233,7 +2263,7 @@
     </row>
     <row r="42" ht="21.5" customHeight="1">
       <c r="A42" t="s" s="10">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B42" t="s" s="11">
         <v>50</v>
@@ -2246,7 +2276,7 @@
     </row>
     <row r="43" ht="21.5" customHeight="1">
       <c r="A43" t="s" s="10">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B43" t="s" s="11">
         <v>51</v>
@@ -2343,7 +2373,7 @@
     </row>
     <row r="48" ht="21.5" customHeight="1">
       <c r="A48" t="s" s="10">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B48" t="s" s="11">
         <v>56</v>
@@ -2356,7 +2386,7 @@
     </row>
     <row r="49" ht="21.5" customHeight="1">
       <c r="A49" t="s" s="10">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B49" t="s" s="11">
         <v>57</v>
@@ -2369,7 +2399,7 @@
     </row>
     <row r="50" ht="21.5" customHeight="1">
       <c r="A50" t="s" s="10">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B50" t="s" s="11">
         <v>58</v>
@@ -2401,7 +2431,7 @@
     </row>
     <row r="52" ht="21.5" customHeight="1">
       <c r="A52" t="s" s="10">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B52" t="s" s="11">
         <v>60</v>
@@ -2414,7 +2444,7 @@
     </row>
     <row r="53" ht="21.5" customHeight="1">
       <c r="A53" t="s" s="10">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B53" t="s" s="11">
         <v>61</v>
@@ -2427,7 +2457,7 @@
     </row>
     <row r="54" ht="21.5" customHeight="1">
       <c r="A54" t="s" s="10">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B54" t="s" s="11">
         <v>62</v>
@@ -2440,7 +2470,7 @@
     </row>
     <row r="55" ht="21.5" customHeight="1">
       <c r="A55" t="s" s="10">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B55" t="s" s="11">
         <v>63</v>
@@ -2474,7 +2504,7 @@
     </row>
     <row r="57" ht="21.5" customHeight="1">
       <c r="A57" t="s" s="10">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B57" t="s" s="11">
         <v>65</v>
@@ -2510,7 +2540,7 @@
     </row>
     <row r="59" ht="21.5" customHeight="1">
       <c r="A59" t="s" s="10">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B59" t="s" s="11">
         <v>67</v>
@@ -2523,7 +2553,7 @@
     </row>
     <row r="60" ht="21.5" customHeight="1">
       <c r="A60" t="s" s="10">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B60" t="s" s="11">
         <v>68</v>
@@ -2536,7 +2566,7 @@
     </row>
     <row r="61" ht="21.5" customHeight="1">
       <c r="A61" t="s" s="10">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B61" t="s" s="11">
         <v>69</v>
@@ -2549,7 +2579,7 @@
     </row>
     <row r="62" ht="21.5" customHeight="1">
       <c r="A62" t="s" s="10">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B62" t="s" s="11">
         <v>70</v>
@@ -2600,7 +2630,7 @@
     </row>
     <row r="65" ht="21.5" customHeight="1">
       <c r="A65" t="s" s="10">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B65" t="s" s="11">
         <v>73</v>
@@ -2634,7 +2664,7 @@
     </row>
     <row r="67" ht="21.5" customHeight="1">
       <c r="A67" t="s" s="10">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B67" t="s" s="11">
         <v>75</v>
@@ -2668,7 +2698,7 @@
     </row>
     <row r="69" ht="21.5" customHeight="1">
       <c r="A69" t="s" s="10">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B69" t="s" s="11">
         <v>77</v>
@@ -2719,7 +2749,7 @@
     </row>
     <row r="72" ht="21.5" customHeight="1">
       <c r="A72" t="s" s="10">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B72" t="s" s="11">
         <v>80</v>
@@ -2791,7 +2821,7 @@
     </row>
     <row r="76" ht="21.5" customHeight="1">
       <c r="A76" t="s" s="10">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B76" t="s" s="11">
         <v>84</v>
@@ -2804,20 +2834,26 @@
     </row>
     <row r="77" ht="21.5" customHeight="1">
       <c r="A77" t="s" s="10">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="B77" t="s" s="11">
         <v>85</v>
       </c>
-      <c r="C77" s="12"/>
-      <c r="D77" s="12"/>
+      <c r="C77" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="D77" t="s" s="11">
+        <v>10</v>
+      </c>
       <c r="E77" s="12"/>
       <c r="F77" s="12"/>
-      <c r="G77" s="12"/>
+      <c r="G77" t="s" s="11">
+        <v>10</v>
+      </c>
     </row>
     <row r="78" ht="21.5" customHeight="1">
       <c r="A78" t="s" s="10">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B78" t="s" s="11">
         <v>86</v>
@@ -2830,7 +2866,7 @@
     </row>
     <row r="79" ht="21.5" customHeight="1">
       <c r="A79" t="s" s="10">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B79" t="s" s="11">
         <v>87</v>
@@ -2866,7 +2902,7 @@
     </row>
     <row r="81" ht="21.5" customHeight="1">
       <c r="A81" t="s" s="10">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B81" t="s" s="11">
         <v>89</v>
@@ -2961,7 +2997,7 @@
     </row>
     <row r="86" ht="21.5" customHeight="1">
       <c r="A86" t="s" s="10">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B86" t="s" s="11">
         <v>94</v>
@@ -2974,20 +3010,28 @@
     </row>
     <row r="87" ht="21.5" customHeight="1">
       <c r="A87" t="s" s="10">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="B87" t="s" s="11">
         <v>95</v>
       </c>
-      <c r="C87" s="12"/>
-      <c r="D87" s="12"/>
-      <c r="E87" s="12"/>
+      <c r="C87" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="D87" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="E87" t="s" s="11">
+        <v>10</v>
+      </c>
       <c r="F87" s="12"/>
-      <c r="G87" s="12"/>
+      <c r="G87" t="s" s="11">
+        <v>10</v>
+      </c>
     </row>
     <row r="88" ht="21.5" customHeight="1">
       <c r="A88" t="s" s="10">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B88" t="s" s="11">
         <v>96</v>

</xml_diff>

<commit_message>
Added butterflies, country, herpetology, macro and moody hubs
</commit_message>
<xml_diff>
--- a/Script Templates/All Hubs.xlsx
+++ b/Script Templates/All Hubs.xlsx
@@ -1943,16 +1943,22 @@
     </row>
     <row r="22" ht="21.5" customHeight="1">
       <c r="A22" t="s" s="10">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B22" t="s" s="11">
         <v>30</v>
       </c>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
+      <c r="C22" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="D22" t="s" s="11">
+        <v>10</v>
+      </c>
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
+      <c r="G22" t="s" s="11">
+        <v>10</v>
+      </c>
     </row>
     <row r="23" ht="21.5" customHeight="1">
       <c r="A23" t="s" s="10">
@@ -2133,16 +2139,22 @@
     </row>
     <row r="34" ht="21.5" customHeight="1">
       <c r="A34" t="s" s="10">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B34" t="s" s="11">
         <v>42</v>
       </c>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
+      <c r="C34" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="D34" t="s" s="11">
+        <v>10</v>
+      </c>
       <c r="E34" s="12"/>
       <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
+      <c r="G34" t="s" s="11">
+        <v>10</v>
+      </c>
     </row>
     <row r="35" ht="21.5" customHeight="1">
       <c r="A35" t="s" s="10">
@@ -2373,16 +2385,24 @@
     </row>
     <row r="48" ht="21.5" customHeight="1">
       <c r="A48" t="s" s="10">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B48" t="s" s="11">
         <v>56</v>
       </c>
-      <c r="C48" s="12"/>
-      <c r="D48" s="12"/>
-      <c r="E48" s="12"/>
+      <c r="C48" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="D48" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="E48" t="s" s="11">
+        <v>10</v>
+      </c>
       <c r="F48" s="12"/>
-      <c r="G48" s="12"/>
+      <c r="G48" t="s" s="11">
+        <v>10</v>
+      </c>
     </row>
     <row r="49" ht="21.5" customHeight="1">
       <c r="A49" t="s" s="10">
@@ -2540,16 +2560,24 @@
     </row>
     <row r="59" ht="21.5" customHeight="1">
       <c r="A59" t="s" s="10">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B59" t="s" s="11">
         <v>67</v>
       </c>
-      <c r="C59" s="12"/>
-      <c r="D59" s="12"/>
-      <c r="E59" s="12"/>
+      <c r="C59" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="D59" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="E59" t="s" s="11">
+        <v>10</v>
+      </c>
       <c r="F59" s="12"/>
-      <c r="G59" s="12"/>
+      <c r="G59" t="s" s="11">
+        <v>10</v>
+      </c>
     </row>
     <row r="60" ht="21.5" customHeight="1">
       <c r="A60" t="s" s="10">
@@ -2579,16 +2607,24 @@
     </row>
     <row r="62" ht="21.5" customHeight="1">
       <c r="A62" t="s" s="10">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B62" t="s" s="11">
         <v>70</v>
       </c>
-      <c r="C62" s="12"/>
-      <c r="D62" s="12"/>
-      <c r="E62" s="12"/>
+      <c r="C62" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="D62" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="E62" t="s" s="11">
+        <v>10</v>
+      </c>
       <c r="F62" s="12"/>
-      <c r="G62" s="12"/>
+      <c r="G62" t="s" s="11">
+        <v>10</v>
+      </c>
     </row>
     <row r="63" ht="21.5" customHeight="1">
       <c r="A63" t="s" s="10">

</xml_diff>

<commit_message>
Added colours, depthoffield, insects, lighthouses and mobile hubs
</commit_message>
<xml_diff>
--- a/Script Templates/All Hubs.xlsx
+++ b/Script Templates/All Hubs.xlsx
@@ -342,7 +342,7 @@
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -358,6 +358,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="12"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="14"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -458,7 +464,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -480,7 +486,7 @@
     <xf numFmtId="49" fontId="4" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -489,13 +495,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -520,6 +529,7 @@
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ff3f3f3f"/>
+      <rgbColor rgb="ff61d836"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1799,7 +1809,7 @@
       </c>
     </row>
     <row r="13" ht="21.5" customHeight="1">
-      <c r="A13" t="s" s="10">
+      <c r="A13" t="s" s="13">
         <v>20</v>
       </c>
       <c r="B13" t="s" s="11">
@@ -1812,7 +1822,7 @@
       <c r="G13" s="12"/>
     </row>
     <row r="14" ht="21.5" customHeight="1">
-      <c r="A14" t="s" s="10">
+      <c r="A14" t="s" s="13">
         <v>20</v>
       </c>
       <c r="B14" t="s" s="11">
@@ -1825,7 +1835,7 @@
       <c r="G14" s="12"/>
     </row>
     <row r="15" ht="21.5" customHeight="1">
-      <c r="A15" t="s" s="10">
+      <c r="A15" t="s" s="13">
         <v>20</v>
       </c>
       <c r="B15" t="s" s="11">
@@ -1876,7 +1886,7 @@
       </c>
     </row>
     <row r="18" ht="21.5" customHeight="1">
-      <c r="A18" t="s" s="10">
+      <c r="A18" t="s" s="13">
         <v>20</v>
       </c>
       <c r="B18" t="s" s="11">
@@ -1930,16 +1940,22 @@
     </row>
     <row r="21" ht="21.5" customHeight="1">
       <c r="A21" t="s" s="10">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B21" t="s" s="11">
         <v>29</v>
       </c>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
+      <c r="C21" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="D21" t="s" s="11">
+        <v>10</v>
+      </c>
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
+      <c r="G21" t="s" s="11">
+        <v>10</v>
+      </c>
     </row>
     <row r="22" ht="21.5" customHeight="1">
       <c r="A22" t="s" s="10">
@@ -1980,7 +1996,7 @@
       </c>
     </row>
     <row r="24" ht="21.5" customHeight="1">
-      <c r="A24" t="s" s="10">
+      <c r="A24" t="s" s="13">
         <v>20</v>
       </c>
       <c r="B24" t="s" s="11">
@@ -1993,7 +2009,7 @@
       <c r="G24" s="12"/>
     </row>
     <row r="25" ht="21.5" customHeight="1">
-      <c r="A25" t="s" s="10">
+      <c r="A25" t="s" s="13">
         <v>20</v>
       </c>
       <c r="B25" t="s" s="11">
@@ -2027,7 +2043,7 @@
       </c>
     </row>
     <row r="27" ht="21.5" customHeight="1">
-      <c r="A27" t="s" s="10">
+      <c r="A27" t="s" s="13">
         <v>20</v>
       </c>
       <c r="B27" t="s" s="11">
@@ -2059,7 +2075,7 @@
       </c>
     </row>
     <row r="29" ht="21.5" customHeight="1">
-      <c r="A29" t="s" s="10">
+      <c r="A29" t="s" s="13">
         <v>20</v>
       </c>
       <c r="B29" t="s" s="11">
@@ -2073,7 +2089,7 @@
     </row>
     <row r="30" ht="21.5" customHeight="1">
       <c r="A30" t="s" s="10">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B30" t="s" s="11">
         <v>38</v>
@@ -2094,19 +2110,25 @@
     </row>
     <row r="31" ht="21.5" customHeight="1">
       <c r="A31" t="s" s="10">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B31" t="s" s="11">
         <v>39</v>
       </c>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
+      <c r="C31" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="D31" t="s" s="11">
+        <v>10</v>
+      </c>
       <c r="E31" s="12"/>
       <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
+      <c r="G31" t="s" s="11">
+        <v>10</v>
+      </c>
     </row>
     <row r="32" ht="21.5" customHeight="1">
-      <c r="A32" t="s" s="10">
+      <c r="A32" t="s" s="13">
         <v>20</v>
       </c>
       <c r="B32" t="s" s="11">
@@ -2179,19 +2201,25 @@
     </row>
     <row r="36" ht="21.5" customHeight="1">
       <c r="A36" t="s" s="10">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B36" t="s" s="11">
         <v>44</v>
       </c>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
+      <c r="C36" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="D36" t="s" s="11">
+        <v>10</v>
+      </c>
       <c r="E36" s="12"/>
       <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
+      <c r="G36" t="s" s="11">
+        <v>10</v>
+      </c>
     </row>
     <row r="37" ht="21.5" customHeight="1">
-      <c r="A37" t="s" s="10">
+      <c r="A37" t="s" s="13">
         <v>20</v>
       </c>
       <c r="B37" t="s" s="11">
@@ -2261,7 +2289,7 @@
       </c>
     </row>
     <row r="41" ht="21.5" customHeight="1">
-      <c r="A41" t="s" s="10">
+      <c r="A41" t="s" s="13">
         <v>20</v>
       </c>
       <c r="B41" t="s" s="11">
@@ -2274,7 +2302,7 @@
       <c r="G41" s="12"/>
     </row>
     <row r="42" ht="21.5" customHeight="1">
-      <c r="A42" t="s" s="10">
+      <c r="A42" t="s" s="13">
         <v>20</v>
       </c>
       <c r="B42" t="s" s="11">
@@ -2287,7 +2315,7 @@
       <c r="G42" s="12"/>
     </row>
     <row r="43" ht="21.5" customHeight="1">
-      <c r="A43" t="s" s="10">
+      <c r="A43" t="s" s="13">
         <v>20</v>
       </c>
       <c r="B43" t="s" s="11">
@@ -2405,7 +2433,7 @@
       </c>
     </row>
     <row r="49" ht="21.5" customHeight="1">
-      <c r="A49" t="s" s="10">
+      <c r="A49" t="s" s="13">
         <v>20</v>
       </c>
       <c r="B49" t="s" s="11">
@@ -2418,7 +2446,7 @@
       <c r="G49" s="12"/>
     </row>
     <row r="50" ht="21.5" customHeight="1">
-      <c r="A50" t="s" s="10">
+      <c r="A50" t="s" s="13">
         <v>20</v>
       </c>
       <c r="B50" t="s" s="11">
@@ -2450,7 +2478,7 @@
       </c>
     </row>
     <row r="52" ht="21.5" customHeight="1">
-      <c r="A52" t="s" s="10">
+      <c r="A52" t="s" s="13">
         <v>20</v>
       </c>
       <c r="B52" t="s" s="11">
@@ -2464,19 +2492,25 @@
     </row>
     <row r="53" ht="21.5" customHeight="1">
       <c r="A53" t="s" s="10">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B53" t="s" s="11">
         <v>61</v>
       </c>
-      <c r="C53" s="12"/>
-      <c r="D53" s="12"/>
+      <c r="C53" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="D53" t="s" s="11">
+        <v>10</v>
+      </c>
       <c r="E53" s="12"/>
       <c r="F53" s="12"/>
-      <c r="G53" s="12"/>
+      <c r="G53" t="s" s="11">
+        <v>10</v>
+      </c>
     </row>
     <row r="54" ht="21.5" customHeight="1">
-      <c r="A54" t="s" s="10">
+      <c r="A54" t="s" s="13">
         <v>20</v>
       </c>
       <c r="B54" t="s" s="11">
@@ -2489,7 +2523,7 @@
       <c r="G54" s="12"/>
     </row>
     <row r="55" ht="21.5" customHeight="1">
-      <c r="A55" t="s" s="10">
+      <c r="A55" t="s" s="13">
         <v>20</v>
       </c>
       <c r="B55" t="s" s="11">
@@ -2524,16 +2558,24 @@
     </row>
     <row r="57" ht="21.5" customHeight="1">
       <c r="A57" t="s" s="10">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B57" t="s" s="11">
         <v>65</v>
       </c>
-      <c r="C57" s="12"/>
-      <c r="D57" s="12"/>
-      <c r="E57" s="12"/>
+      <c r="C57" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="D57" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="E57" t="s" s="11">
+        <v>10</v>
+      </c>
       <c r="F57" s="12"/>
-      <c r="G57" s="12"/>
+      <c r="G57" t="s" s="11">
+        <v>10</v>
+      </c>
     </row>
     <row r="58" ht="21.5" customHeight="1">
       <c r="A58" t="s" s="10">
@@ -2580,7 +2622,7 @@
       </c>
     </row>
     <row r="60" ht="21.5" customHeight="1">
-      <c r="A60" t="s" s="10">
+      <c r="A60" t="s" s="13">
         <v>20</v>
       </c>
       <c r="B60" t="s" s="11">
@@ -2594,16 +2636,24 @@
     </row>
     <row r="61" ht="21.5" customHeight="1">
       <c r="A61" t="s" s="10">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B61" t="s" s="11">
         <v>69</v>
       </c>
-      <c r="C61" s="12"/>
-      <c r="D61" s="12"/>
-      <c r="E61" s="12"/>
+      <c r="C61" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="D61" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="E61" t="s" s="11">
+        <v>10</v>
+      </c>
       <c r="F61" s="12"/>
-      <c r="G61" s="12"/>
+      <c r="G61" t="s" s="11">
+        <v>10</v>
+      </c>
     </row>
     <row r="62" ht="21.5" customHeight="1">
       <c r="A62" t="s" s="10">
@@ -2665,7 +2715,7 @@
       </c>
     </row>
     <row r="65" ht="21.5" customHeight="1">
-      <c r="A65" t="s" s="10">
+      <c r="A65" t="s" s="13">
         <v>20</v>
       </c>
       <c r="B65" t="s" s="11">
@@ -2699,7 +2749,7 @@
       </c>
     </row>
     <row r="67" ht="21.5" customHeight="1">
-      <c r="A67" t="s" s="10">
+      <c r="A67" t="s" s="13">
         <v>20</v>
       </c>
       <c r="B67" t="s" s="11">
@@ -2733,7 +2783,7 @@
       </c>
     </row>
     <row r="69" ht="21.5" customHeight="1">
-      <c r="A69" t="s" s="10">
+      <c r="A69" t="s" s="13">
         <v>20</v>
       </c>
       <c r="B69" t="s" s="11">
@@ -2784,7 +2834,7 @@
       </c>
     </row>
     <row r="72" ht="21.5" customHeight="1">
-      <c r="A72" t="s" s="10">
+      <c r="A72" t="s" s="13">
         <v>20</v>
       </c>
       <c r="B72" t="s" s="11">
@@ -2856,7 +2906,7 @@
       </c>
     </row>
     <row r="76" ht="21.5" customHeight="1">
-      <c r="A76" t="s" s="10">
+      <c r="A76" t="s" s="13">
         <v>20</v>
       </c>
       <c r="B76" t="s" s="11">
@@ -2888,7 +2938,7 @@
       </c>
     </row>
     <row r="78" ht="21.5" customHeight="1">
-      <c r="A78" t="s" s="10">
+      <c r="A78" t="s" s="13">
         <v>20</v>
       </c>
       <c r="B78" t="s" s="11">
@@ -2901,7 +2951,7 @@
       <c r="G78" s="12"/>
     </row>
     <row r="79" ht="21.5" customHeight="1">
-      <c r="A79" t="s" s="10">
+      <c r="A79" t="s" s="13">
         <v>20</v>
       </c>
       <c r="B79" t="s" s="11">
@@ -2937,7 +2987,7 @@
       </c>
     </row>
     <row r="81" ht="21.5" customHeight="1">
-      <c r="A81" t="s" s="10">
+      <c r="A81" t="s" s="13">
         <v>20</v>
       </c>
       <c r="B81" t="s" s="11">
@@ -3032,7 +3082,7 @@
       </c>
     </row>
     <row r="86" ht="21.5" customHeight="1">
-      <c r="A86" t="s" s="10">
+      <c r="A86" t="s" s="13">
         <v>20</v>
       </c>
       <c r="B86" t="s" s="11">
@@ -3066,7 +3116,7 @@
       </c>
     </row>
     <row r="88" ht="21.5" customHeight="1">
-      <c r="A88" t="s" s="10">
+      <c r="A88" t="s" s="13">
         <v>20</v>
       </c>
       <c r="B88" t="s" s="11">

</xml_diff>

<commit_message>
added flowers and hikes hubs
</commit_message>
<xml_diff>
--- a/Script Templates/All Hubs.xlsx
+++ b/Script Templates/All Hubs.xlsx
@@ -2315,17 +2315,23 @@
       <c r="G42" s="12"/>
     </row>
     <row r="43" ht="21.5" customHeight="1">
-      <c r="A43" t="s" s="13">
-        <v>20</v>
+      <c r="A43" t="s" s="10">
+        <v>8</v>
       </c>
       <c r="B43" t="s" s="11">
         <v>51</v>
       </c>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
+      <c r="C43" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="D43" t="s" s="11">
+        <v>10</v>
+      </c>
       <c r="E43" s="12"/>
       <c r="F43" s="12"/>
-      <c r="G43" s="12"/>
+      <c r="G43" t="s" s="11">
+        <v>10</v>
+      </c>
     </row>
     <row r="44" ht="21.5" customHeight="1">
       <c r="A44" t="s" s="10">
@@ -2433,17 +2439,23 @@
       </c>
     </row>
     <row r="49" ht="21.5" customHeight="1">
-      <c r="A49" t="s" s="13">
-        <v>20</v>
+      <c r="A49" t="s" s="10">
+        <v>8</v>
       </c>
       <c r="B49" t="s" s="11">
         <v>57</v>
       </c>
-      <c r="C49" s="12"/>
-      <c r="D49" s="12"/>
+      <c r="C49" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="D49" t="s" s="11">
+        <v>10</v>
+      </c>
       <c r="E49" s="12"/>
       <c r="F49" s="12"/>
-      <c r="G49" s="12"/>
+      <c r="G49" t="s" s="11">
+        <v>10</v>
+      </c>
     </row>
     <row r="50" ht="21.5" customHeight="1">
       <c r="A50" t="s" s="13">

</xml_diff>

<commit_message>
Added the artgallery, asia, australia, blue, cats, china, cocktails, collage and drone hubs
</commit_message>
<xml_diff>
--- a/Script Templates/All Hubs.xlsx
+++ b/Script Templates/All Hubs.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="100">
   <si>
     <t>Hubs Script Templates</t>
   </si>
@@ -73,91 +73,97 @@
     <t>architecture</t>
   </si>
   <si>
+    <t>artgallery</t>
+  </si>
+  <si>
+    <t>asia</t>
+  </si>
+  <si>
+    <t>australia</t>
+  </si>
+  <si>
+    <t>beaches</t>
+  </si>
+  <si>
+    <t>birds</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>bnw</t>
+  </si>
+  <si>
+    <t>books</t>
+  </si>
+  <si>
+    <t>bridges</t>
+  </si>
+  <si>
+    <t>butterflies</t>
+  </si>
+  <si>
+    <t>canada</t>
+  </si>
+  <si>
+    <t>cats</t>
+  </si>
+  <si>
+    <t>china</t>
+  </si>
+  <si>
+    <t>cityscape</t>
+  </si>
+  <si>
+    <t>cocktails</t>
+  </si>
+  <si>
+    <t>coffee</t>
+  </si>
+  <si>
+    <t>collage</t>
+  </si>
+  <si>
+    <t>colorsplash</t>
+  </si>
+  <si>
+    <t>colours</t>
+  </si>
+  <si>
+    <t>NOT FEATURE HUB</t>
+  </si>
+  <si>
+    <t>community</t>
+  </si>
+  <si>
+    <t>—</t>
+  </si>
+  <si>
+    <t>community_member</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>cuteness</t>
+  </si>
+  <si>
+    <t>depthoffield</t>
+  </si>
+  <si>
+    <t>drone</t>
+  </si>
+  <si>
+    <t>drops</t>
+  </si>
+  <si>
+    <t>edit</t>
+  </si>
+  <si>
+    <t>europe</t>
+  </si>
+  <si>
     <t xml:space="preserve">[ ] </t>
-  </si>
-  <si>
-    <t>artgallery</t>
-  </si>
-  <si>
-    <t>asia</t>
-  </si>
-  <si>
-    <t>australia</t>
-  </si>
-  <si>
-    <t>beaches</t>
-  </si>
-  <si>
-    <t>birds</t>
-  </si>
-  <si>
-    <t>blue</t>
-  </si>
-  <si>
-    <t>bnw</t>
-  </si>
-  <si>
-    <t>books</t>
-  </si>
-  <si>
-    <t>bridges</t>
-  </si>
-  <si>
-    <t>butterflies</t>
-  </si>
-  <si>
-    <t>canada</t>
-  </si>
-  <si>
-    <t>cats</t>
-  </si>
-  <si>
-    <t>china</t>
-  </si>
-  <si>
-    <t>cityscape</t>
-  </si>
-  <si>
-    <t>cocktails</t>
-  </si>
-  <si>
-    <t>coffee</t>
-  </si>
-  <si>
-    <t>collage</t>
-  </si>
-  <si>
-    <t>colorsplash</t>
-  </si>
-  <si>
-    <t>colours</t>
-  </si>
-  <si>
-    <t>community</t>
-  </si>
-  <si>
-    <t>community_member</t>
-  </si>
-  <si>
-    <t>country</t>
-  </si>
-  <si>
-    <t>cuteness</t>
-  </si>
-  <si>
-    <t>depthoffield</t>
-  </si>
-  <si>
-    <t>drone</t>
-  </si>
-  <si>
-    <t>drops</t>
-  </si>
-  <si>
-    <t>edit</t>
-  </si>
-  <si>
-    <t>europe</t>
   </si>
   <si>
     <t>fishing</t>
@@ -342,7 +348,7 @@
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -364,6 +370,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="14"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="15"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -464,7 +476,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -504,6 +516,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -530,6 +545,7 @@
       <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ff61d836"/>
+      <rgbColor rgb="ffff8a7a"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1809,50 +1825,70 @@
       </c>
     </row>
     <row r="13" ht="21.5" customHeight="1">
-      <c r="A13" t="s" s="13">
+      <c r="A13" t="s" s="10">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s" s="11">
         <v>20</v>
       </c>
-      <c r="B13" t="s" s="11">
-        <v>21</v>
-      </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
+      <c r="C13" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s" s="11">
+        <v>10</v>
+      </c>
       <c r="E13" s="12"/>
       <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
+      <c r="G13" t="s" s="11">
+        <v>10</v>
+      </c>
     </row>
     <row r="14" ht="21.5" customHeight="1">
-      <c r="A14" t="s" s="13">
-        <v>20</v>
+      <c r="A14" t="s" s="10">
+        <v>8</v>
       </c>
       <c r="B14" t="s" s="11">
-        <v>22</v>
-      </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
+        <v>21</v>
+      </c>
+      <c r="C14" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s" s="11">
+        <v>10</v>
+      </c>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
+      <c r="G14" t="s" s="11">
+        <v>10</v>
+      </c>
     </row>
     <row r="15" ht="21.5" customHeight="1">
-      <c r="A15" t="s" s="13">
-        <v>20</v>
+      <c r="A15" t="s" s="10">
+        <v>8</v>
       </c>
       <c r="B15" t="s" s="11">
-        <v>23</v>
-      </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
+        <v>22</v>
+      </c>
+      <c r="C15" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="E15" t="s" s="11">
+        <v>10</v>
+      </c>
       <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
+      <c r="G15" t="s" s="11">
+        <v>10</v>
+      </c>
     </row>
     <row r="16" ht="21.5" customHeight="1">
       <c r="A16" t="s" s="10">
         <v>8</v>
       </c>
       <c r="B16" t="s" s="11">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s" s="11">
         <v>10</v>
@@ -1871,7 +1907,7 @@
         <v>8</v>
       </c>
       <c r="B17" t="s" s="11">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s" s="11">
         <v>10</v>
@@ -1886,24 +1922,30 @@
       </c>
     </row>
     <row r="18" ht="21.5" customHeight="1">
-      <c r="A18" t="s" s="13">
-        <v>20</v>
+      <c r="A18" t="s" s="10">
+        <v>8</v>
       </c>
       <c r="B18" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
+        <v>25</v>
+      </c>
+      <c r="C18" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="D18" t="s" s="11">
+        <v>10</v>
+      </c>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
+      <c r="G18" t="s" s="11">
+        <v>10</v>
+      </c>
     </row>
     <row r="19" ht="21.5" customHeight="1">
       <c r="A19" t="s" s="10">
         <v>8</v>
       </c>
       <c r="B19" t="s" s="11">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C19" t="s" s="11">
         <v>10</v>
@@ -1924,7 +1966,7 @@
         <v>8</v>
       </c>
       <c r="B20" t="s" s="11">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C20" t="s" s="11">
         <v>10</v>
@@ -1943,7 +1985,7 @@
         <v>8</v>
       </c>
       <c r="B21" t="s" s="11">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C21" t="s" s="11">
         <v>10</v>
@@ -1962,7 +2004,7 @@
         <v>8</v>
       </c>
       <c r="B22" t="s" s="11">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C22" t="s" s="11">
         <v>10</v>
@@ -1981,7 +2023,7 @@
         <v>8</v>
       </c>
       <c r="B23" t="s" s="11">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C23" t="s" s="11">
         <v>10</v>
@@ -1996,37 +2038,49 @@
       </c>
     </row>
     <row r="24" ht="21.5" customHeight="1">
-      <c r="A24" t="s" s="13">
-        <v>20</v>
+      <c r="A24" t="s" s="10">
+        <v>8</v>
       </c>
       <c r="B24" t="s" s="11">
-        <v>32</v>
-      </c>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
+        <v>31</v>
+      </c>
+      <c r="C24" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="D24" t="s" s="11">
+        <v>10</v>
+      </c>
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
+      <c r="G24" t="s" s="11">
+        <v>10</v>
+      </c>
     </row>
     <row r="25" ht="21.5" customHeight="1">
-      <c r="A25" t="s" s="13">
-        <v>20</v>
+      <c r="A25" t="s" s="10">
+        <v>8</v>
       </c>
       <c r="B25" t="s" s="11">
-        <v>33</v>
-      </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
+        <v>32</v>
+      </c>
+      <c r="C25" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="D25" t="s" s="11">
+        <v>10</v>
+      </c>
       <c r="E25" s="12"/>
       <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
+      <c r="G25" t="s" s="11">
+        <v>10</v>
+      </c>
     </row>
     <row r="26" ht="21.5" customHeight="1">
       <c r="A26" t="s" s="10">
         <v>8</v>
       </c>
       <c r="B26" t="s" s="11">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C26" t="s" s="11">
         <v>10</v>
@@ -2043,24 +2097,30 @@
       </c>
     </row>
     <row r="27" ht="21.5" customHeight="1">
-      <c r="A27" t="s" s="13">
-        <v>20</v>
+      <c r="A27" t="s" s="10">
+        <v>8</v>
       </c>
       <c r="B27" t="s" s="11">
-        <v>35</v>
-      </c>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
+        <v>34</v>
+      </c>
+      <c r="C27" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="D27" t="s" s="11">
+        <v>10</v>
+      </c>
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
+      <c r="G27" t="s" s="11">
+        <v>10</v>
+      </c>
     </row>
     <row r="28" ht="21.5" customHeight="1">
       <c r="A28" t="s" s="10">
         <v>8</v>
       </c>
       <c r="B28" t="s" s="11">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C28" t="s" s="11">
         <v>10</v>
@@ -2075,24 +2135,30 @@
       </c>
     </row>
     <row r="29" ht="21.5" customHeight="1">
-      <c r="A29" t="s" s="13">
-        <v>20</v>
+      <c r="A29" t="s" s="10">
+        <v>8</v>
       </c>
       <c r="B29" t="s" s="11">
-        <v>37</v>
-      </c>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
+        <v>36</v>
+      </c>
+      <c r="C29" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="D29" t="s" s="11">
+        <v>10</v>
+      </c>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
+      <c r="G29" t="s" s="11">
+        <v>10</v>
+      </c>
     </row>
     <row r="30" ht="21.5" customHeight="1">
       <c r="A30" t="s" s="10">
         <v>8</v>
       </c>
       <c r="B30" t="s" s="11">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C30" t="s" s="11">
         <v>10</v>
@@ -2113,7 +2179,7 @@
         <v>8</v>
       </c>
       <c r="B31" t="s" s="11">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C31" t="s" s="11">
         <v>10</v>
@@ -2129,23 +2195,33 @@
     </row>
     <row r="32" ht="21.5" customHeight="1">
       <c r="A32" t="s" s="13">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="B32" t="s" s="11">
         <v>40</v>
       </c>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12"/>
+      <c r="C32" t="s" s="11">
+        <v>41</v>
+      </c>
+      <c r="D32" t="s" s="11">
+        <v>41</v>
+      </c>
+      <c r="E32" t="s" s="11">
+        <v>41</v>
+      </c>
+      <c r="F32" t="s" s="11">
+        <v>41</v>
+      </c>
+      <c r="G32" t="s" s="11">
+        <v>41</v>
+      </c>
     </row>
     <row r="33" ht="21.5" customHeight="1">
       <c r="A33" t="s" s="10">
         <v>8</v>
       </c>
       <c r="B33" t="s" s="11">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C33" t="s" s="11">
         <v>10</v>
@@ -2164,7 +2240,7 @@
         <v>8</v>
       </c>
       <c r="B34" t="s" s="11">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C34" t="s" s="11">
         <v>10</v>
@@ -2183,7 +2259,7 @@
         <v>8</v>
       </c>
       <c r="B35" t="s" s="11">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C35" t="s" s="11">
         <v>10</v>
@@ -2204,7 +2280,7 @@
         <v>8</v>
       </c>
       <c r="B36" t="s" s="11">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C36" t="s" s="11">
         <v>10</v>
@@ -2219,24 +2295,32 @@
       </c>
     </row>
     <row r="37" ht="21.5" customHeight="1">
-      <c r="A37" t="s" s="13">
-        <v>20</v>
+      <c r="A37" t="s" s="10">
+        <v>8</v>
       </c>
       <c r="B37" t="s" s="11">
-        <v>45</v>
-      </c>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="12"/>
+        <v>46</v>
+      </c>
+      <c r="C37" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="D37" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="E37" t="s" s="11">
+        <v>10</v>
+      </c>
       <c r="F37" s="12"/>
-      <c r="G37" s="12"/>
+      <c r="G37" t="s" s="11">
+        <v>10</v>
+      </c>
     </row>
     <row r="38" ht="21.5" customHeight="1">
       <c r="A38" t="s" s="10">
         <v>8</v>
       </c>
       <c r="B38" t="s" s="11">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C38" t="s" s="11">
         <v>10</v>
@@ -2255,7 +2339,7 @@
         <v>8</v>
       </c>
       <c r="B39" t="s" s="11">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C39" t="s" s="11">
         <v>10</v>
@@ -2274,7 +2358,7 @@
         <v>8</v>
       </c>
       <c r="B40" t="s" s="11">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C40" t="s" s="11">
         <v>10</v>
@@ -2289,11 +2373,11 @@
       </c>
     </row>
     <row r="41" ht="21.5" customHeight="1">
-      <c r="A41" t="s" s="13">
-        <v>20</v>
+      <c r="A41" t="s" s="14">
+        <v>50</v>
       </c>
       <c r="B41" t="s" s="11">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C41" s="12"/>
       <c r="D41" s="12"/>
@@ -2302,11 +2386,11 @@
       <c r="G41" s="12"/>
     </row>
     <row r="42" ht="21.5" customHeight="1">
-      <c r="A42" t="s" s="13">
-        <v>20</v>
+      <c r="A42" t="s" s="14">
+        <v>50</v>
       </c>
       <c r="B42" t="s" s="11">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C42" s="12"/>
       <c r="D42" s="12"/>
@@ -2319,7 +2403,7 @@
         <v>8</v>
       </c>
       <c r="B43" t="s" s="11">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C43" t="s" s="11">
         <v>10</v>
@@ -2338,7 +2422,7 @@
         <v>8</v>
       </c>
       <c r="B44" t="s" s="11">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C44" t="s" s="11">
         <v>10</v>
@@ -2359,7 +2443,7 @@
         <v>8</v>
       </c>
       <c r="B45" t="s" s="11">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C45" t="s" s="11">
         <v>10</v>
@@ -2380,7 +2464,7 @@
         <v>8</v>
       </c>
       <c r="B46" t="s" s="11">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C46" t="s" s="11">
         <v>10</v>
@@ -2403,7 +2487,7 @@
         <v>8</v>
       </c>
       <c r="B47" t="s" s="11">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C47" t="s" s="11">
         <v>10</v>
@@ -2422,7 +2506,7 @@
         <v>8</v>
       </c>
       <c r="B48" t="s" s="11">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C48" t="s" s="11">
         <v>10</v>
@@ -2443,7 +2527,7 @@
         <v>8</v>
       </c>
       <c r="B49" t="s" s="11">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C49" t="s" s="11">
         <v>10</v>
@@ -2458,11 +2542,11 @@
       </c>
     </row>
     <row r="50" ht="21.5" customHeight="1">
-      <c r="A50" t="s" s="13">
-        <v>20</v>
+      <c r="A50" t="s" s="14">
+        <v>50</v>
       </c>
       <c r="B50" t="s" s="11">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C50" s="12"/>
       <c r="D50" s="12"/>
@@ -2475,7 +2559,7 @@
         <v>8</v>
       </c>
       <c r="B51" t="s" s="11">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C51" t="s" s="11">
         <v>10</v>
@@ -2490,11 +2574,11 @@
       </c>
     </row>
     <row r="52" ht="21.5" customHeight="1">
-      <c r="A52" t="s" s="13">
-        <v>20</v>
+      <c r="A52" t="s" s="14">
+        <v>50</v>
       </c>
       <c r="B52" t="s" s="11">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C52" s="12"/>
       <c r="D52" s="12"/>
@@ -2507,7 +2591,7 @@
         <v>8</v>
       </c>
       <c r="B53" t="s" s="11">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C53" t="s" s="11">
         <v>10</v>
@@ -2522,11 +2606,11 @@
       </c>
     </row>
     <row r="54" ht="21.5" customHeight="1">
-      <c r="A54" t="s" s="13">
-        <v>20</v>
+      <c r="A54" t="s" s="14">
+        <v>50</v>
       </c>
       <c r="B54" t="s" s="11">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C54" s="12"/>
       <c r="D54" s="12"/>
@@ -2535,11 +2619,11 @@
       <c r="G54" s="12"/>
     </row>
     <row r="55" ht="21.5" customHeight="1">
-      <c r="A55" t="s" s="13">
-        <v>20</v>
+      <c r="A55" t="s" s="14">
+        <v>50</v>
       </c>
       <c r="B55" t="s" s="11">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C55" s="12"/>
       <c r="D55" s="12"/>
@@ -2552,7 +2636,7 @@
         <v>8</v>
       </c>
       <c r="B56" t="s" s="11">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C56" t="s" s="11">
         <v>10</v>
@@ -2573,7 +2657,7 @@
         <v>8</v>
       </c>
       <c r="B57" t="s" s="11">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C57" t="s" s="11">
         <v>10</v>
@@ -2594,7 +2678,7 @@
         <v>8</v>
       </c>
       <c r="B58" t="s" s="11">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C58" t="s" s="11">
         <v>10</v>
@@ -2617,7 +2701,7 @@
         <v>8</v>
       </c>
       <c r="B59" t="s" s="11">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C59" t="s" s="11">
         <v>10</v>
@@ -2634,11 +2718,11 @@
       </c>
     </row>
     <row r="60" ht="21.5" customHeight="1">
-      <c r="A60" t="s" s="13">
-        <v>20</v>
+      <c r="A60" t="s" s="14">
+        <v>50</v>
       </c>
       <c r="B60" t="s" s="11">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C60" s="12"/>
       <c r="D60" s="12"/>
@@ -2651,7 +2735,7 @@
         <v>8</v>
       </c>
       <c r="B61" t="s" s="11">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C61" t="s" s="11">
         <v>10</v>
@@ -2672,7 +2756,7 @@
         <v>8</v>
       </c>
       <c r="B62" t="s" s="11">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C62" t="s" s="11">
         <v>10</v>
@@ -2693,7 +2777,7 @@
         <v>8</v>
       </c>
       <c r="B63" t="s" s="11">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C63" t="s" s="11">
         <v>10</v>
@@ -2712,7 +2796,7 @@
         <v>8</v>
       </c>
       <c r="B64" t="s" s="11">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C64" t="s" s="11">
         <v>10</v>
@@ -2727,11 +2811,11 @@
       </c>
     </row>
     <row r="65" ht="21.5" customHeight="1">
-      <c r="A65" t="s" s="13">
-        <v>20</v>
+      <c r="A65" t="s" s="14">
+        <v>50</v>
       </c>
       <c r="B65" t="s" s="11">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C65" s="12"/>
       <c r="D65" s="12"/>
@@ -2744,7 +2828,7 @@
         <v>8</v>
       </c>
       <c r="B66" t="s" s="11">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C66" t="s" s="11">
         <v>10</v>
@@ -2761,11 +2845,11 @@
       </c>
     </row>
     <row r="67" ht="21.5" customHeight="1">
-      <c r="A67" t="s" s="13">
-        <v>20</v>
+      <c r="A67" t="s" s="14">
+        <v>50</v>
       </c>
       <c r="B67" t="s" s="11">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C67" s="12"/>
       <c r="D67" s="12"/>
@@ -2778,7 +2862,7 @@
         <v>8</v>
       </c>
       <c r="B68" t="s" s="11">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C68" t="s" s="11">
         <v>10</v>
@@ -2795,11 +2879,11 @@
       </c>
     </row>
     <row r="69" ht="21.5" customHeight="1">
-      <c r="A69" t="s" s="13">
-        <v>20</v>
+      <c r="A69" t="s" s="14">
+        <v>50</v>
       </c>
       <c r="B69" t="s" s="11">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C69" s="12"/>
       <c r="D69" s="12"/>
@@ -2812,7 +2896,7 @@
         <v>8</v>
       </c>
       <c r="B70" t="s" s="11">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C70" t="s" s="11">
         <v>10</v>
@@ -2831,7 +2915,7 @@
         <v>8</v>
       </c>
       <c r="B71" t="s" s="11">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C71" t="s" s="11">
         <v>10</v>
@@ -2846,11 +2930,11 @@
       </c>
     </row>
     <row r="72" ht="21.5" customHeight="1">
-      <c r="A72" t="s" s="13">
-        <v>20</v>
+      <c r="A72" t="s" s="14">
+        <v>50</v>
       </c>
       <c r="B72" t="s" s="11">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C72" s="12"/>
       <c r="D72" s="12"/>
@@ -2863,7 +2947,7 @@
         <v>8</v>
       </c>
       <c r="B73" t="s" s="11">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C73" t="s" s="11">
         <v>10</v>
@@ -2882,7 +2966,7 @@
         <v>8</v>
       </c>
       <c r="B74" t="s" s="11">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C74" t="s" s="11">
         <v>10</v>
@@ -2901,7 +2985,7 @@
         <v>8</v>
       </c>
       <c r="B75" t="s" s="11">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C75" t="s" s="11">
         <v>10</v>
@@ -2918,11 +3002,11 @@
       </c>
     </row>
     <row r="76" ht="21.5" customHeight="1">
-      <c r="A76" t="s" s="13">
-        <v>20</v>
+      <c r="A76" t="s" s="14">
+        <v>50</v>
       </c>
       <c r="B76" t="s" s="11">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C76" s="12"/>
       <c r="D76" s="12"/>
@@ -2935,7 +3019,7 @@
         <v>8</v>
       </c>
       <c r="B77" t="s" s="11">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C77" t="s" s="11">
         <v>10</v>
@@ -2950,11 +3034,11 @@
       </c>
     </row>
     <row r="78" ht="21.5" customHeight="1">
-      <c r="A78" t="s" s="13">
-        <v>20</v>
+      <c r="A78" t="s" s="14">
+        <v>50</v>
       </c>
       <c r="B78" t="s" s="11">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C78" s="12"/>
       <c r="D78" s="12"/>
@@ -2963,11 +3047,11 @@
       <c r="G78" s="12"/>
     </row>
     <row r="79" ht="21.5" customHeight="1">
-      <c r="A79" t="s" s="13">
-        <v>20</v>
+      <c r="A79" t="s" s="14">
+        <v>50</v>
       </c>
       <c r="B79" t="s" s="11">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C79" s="12"/>
       <c r="D79" s="12"/>
@@ -2980,7 +3064,7 @@
         <v>8</v>
       </c>
       <c r="B80" t="s" s="11">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C80" t="s" s="11">
         <v>10</v>
@@ -2999,11 +3083,11 @@
       </c>
     </row>
     <row r="81" ht="21.5" customHeight="1">
-      <c r="A81" t="s" s="13">
-        <v>20</v>
+      <c r="A81" t="s" s="14">
+        <v>50</v>
       </c>
       <c r="B81" t="s" s="11">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C81" s="12"/>
       <c r="D81" s="12"/>
@@ -3016,7 +3100,7 @@
         <v>8</v>
       </c>
       <c r="B82" t="s" s="11">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C82" t="s" s="11">
         <v>10</v>
@@ -3039,7 +3123,7 @@
         <v>8</v>
       </c>
       <c r="B83" t="s" s="11">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C83" t="s" s="11">
         <v>10</v>
@@ -3060,7 +3144,7 @@
         <v>8</v>
       </c>
       <c r="B84" t="s" s="11">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C84" t="s" s="11">
         <v>10</v>
@@ -3079,7 +3163,7 @@
         <v>8</v>
       </c>
       <c r="B85" t="s" s="11">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C85" t="s" s="11">
         <v>10</v>
@@ -3094,11 +3178,11 @@
       </c>
     </row>
     <row r="86" ht="21.5" customHeight="1">
-      <c r="A86" t="s" s="13">
-        <v>20</v>
+      <c r="A86" t="s" s="14">
+        <v>50</v>
       </c>
       <c r="B86" t="s" s="11">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C86" s="12"/>
       <c r="D86" s="12"/>
@@ -3111,7 +3195,7 @@
         <v>8</v>
       </c>
       <c r="B87" t="s" s="11">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C87" t="s" s="11">
         <v>10</v>
@@ -3128,11 +3212,11 @@
       </c>
     </row>
     <row r="88" ht="21.5" customHeight="1">
-      <c r="A88" t="s" s="13">
-        <v>20</v>
+      <c r="A88" t="s" s="14">
+        <v>50</v>
       </c>
       <c r="B88" t="s" s="11">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C88" s="12"/>
       <c r="D88" s="12"/>
@@ -3145,7 +3229,7 @@
         <v>8</v>
       </c>
       <c r="B89" t="s" s="11">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C89" t="s" s="11">
         <v>10</v>

</xml_diff>

<commit_message>
Finishing all the hubs
</commit_message>
<xml_diff>
--- a/Script Templates/All Hubs.xlsx
+++ b/Script Templates/All Hubs.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="99">
   <si>
     <t>Hubs Script Templates</t>
   </si>
@@ -161,9 +161,6 @@
   </si>
   <si>
     <t>europe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ ] </t>
   </si>
   <si>
     <t>fishing</t>
@@ -476,7 +473,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -517,9 +514,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="5" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2373,37 +2367,53 @@
       </c>
     </row>
     <row r="41" ht="21.5" customHeight="1">
-      <c r="A41" t="s" s="14">
+      <c r="A41" t="s" s="10">
+        <v>8</v>
+      </c>
+      <c r="B41" t="s" s="11">
         <v>50</v>
       </c>
-      <c r="B41" t="s" s="11">
+      <c r="C41" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="D41" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="E41" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="F41" s="12"/>
+      <c r="G41" t="s" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" ht="21.5" customHeight="1">
+      <c r="A42" t="s" s="10">
+        <v>8</v>
+      </c>
+      <c r="B42" t="s" s="11">
         <v>51</v>
       </c>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="12"/>
-    </row>
-    <row r="42" ht="21.5" customHeight="1">
-      <c r="A42" t="s" s="14">
-        <v>50</v>
-      </c>
-      <c r="B42" t="s" s="11">
-        <v>52</v>
-      </c>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
+      <c r="C42" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="D42" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="E42" t="s" s="11">
+        <v>10</v>
+      </c>
       <c r="F42" s="12"/>
-      <c r="G42" s="12"/>
+      <c r="G42" t="s" s="11">
+        <v>10</v>
+      </c>
     </row>
     <row r="43" ht="21.5" customHeight="1">
       <c r="A43" t="s" s="10">
         <v>8</v>
       </c>
       <c r="B43" t="s" s="11">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C43" t="s" s="11">
         <v>10</v>
@@ -2422,7 +2432,7 @@
         <v>8</v>
       </c>
       <c r="B44" t="s" s="11">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C44" t="s" s="11">
         <v>10</v>
@@ -2443,7 +2453,7 @@
         <v>8</v>
       </c>
       <c r="B45" t="s" s="11">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C45" t="s" s="11">
         <v>10</v>
@@ -2464,7 +2474,7 @@
         <v>8</v>
       </c>
       <c r="B46" t="s" s="11">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C46" t="s" s="11">
         <v>10</v>
@@ -2487,7 +2497,7 @@
         <v>8</v>
       </c>
       <c r="B47" t="s" s="11">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C47" t="s" s="11">
         <v>10</v>
@@ -2506,7 +2516,7 @@
         <v>8</v>
       </c>
       <c r="B48" t="s" s="11">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C48" t="s" s="11">
         <v>10</v>
@@ -2527,7 +2537,7 @@
         <v>8</v>
       </c>
       <c r="B49" t="s" s="11">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C49" t="s" s="11">
         <v>10</v>
@@ -2542,24 +2552,32 @@
       </c>
     </row>
     <row r="50" ht="21.5" customHeight="1">
-      <c r="A50" t="s" s="14">
-        <v>50</v>
+      <c r="A50" t="s" s="10">
+        <v>8</v>
       </c>
       <c r="B50" t="s" s="11">
-        <v>60</v>
-      </c>
-      <c r="C50" s="12"/>
-      <c r="D50" s="12"/>
-      <c r="E50" s="12"/>
+        <v>59</v>
+      </c>
+      <c r="C50" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="D50" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="E50" t="s" s="11">
+        <v>10</v>
+      </c>
       <c r="F50" s="12"/>
-      <c r="G50" s="12"/>
+      <c r="G50" t="s" s="11">
+        <v>10</v>
+      </c>
     </row>
     <row r="51" ht="21.5" customHeight="1">
       <c r="A51" t="s" s="10">
         <v>8</v>
       </c>
       <c r="B51" t="s" s="11">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C51" t="s" s="11">
         <v>10</v>
@@ -2574,24 +2592,30 @@
       </c>
     </row>
     <row r="52" ht="21.5" customHeight="1">
-      <c r="A52" t="s" s="14">
-        <v>50</v>
+      <c r="A52" t="s" s="10">
+        <v>8</v>
       </c>
       <c r="B52" t="s" s="11">
-        <v>62</v>
-      </c>
-      <c r="C52" s="12"/>
-      <c r="D52" s="12"/>
+        <v>61</v>
+      </c>
+      <c r="C52" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="D52" t="s" s="11">
+        <v>10</v>
+      </c>
       <c r="E52" s="12"/>
       <c r="F52" s="12"/>
-      <c r="G52" s="12"/>
+      <c r="G52" t="s" s="11">
+        <v>10</v>
+      </c>
     </row>
     <row r="53" ht="21.5" customHeight="1">
       <c r="A53" t="s" s="10">
         <v>8</v>
       </c>
       <c r="B53" t="s" s="11">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C53" t="s" s="11">
         <v>10</v>
@@ -2606,37 +2630,51 @@
       </c>
     </row>
     <row r="54" ht="21.5" customHeight="1">
-      <c r="A54" t="s" s="14">
-        <v>50</v>
+      <c r="A54" t="s" s="10">
+        <v>8</v>
       </c>
       <c r="B54" t="s" s="11">
-        <v>64</v>
-      </c>
-      <c r="C54" s="12"/>
-      <c r="D54" s="12"/>
+        <v>63</v>
+      </c>
+      <c r="C54" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="D54" t="s" s="11">
+        <v>10</v>
+      </c>
       <c r="E54" s="12"/>
       <c r="F54" s="12"/>
-      <c r="G54" s="12"/>
+      <c r="G54" t="s" s="11">
+        <v>10</v>
+      </c>
     </row>
     <row r="55" ht="21.5" customHeight="1">
-      <c r="A55" t="s" s="14">
-        <v>50</v>
+      <c r="A55" t="s" s="10">
+        <v>8</v>
       </c>
       <c r="B55" t="s" s="11">
-        <v>65</v>
-      </c>
-      <c r="C55" s="12"/>
-      <c r="D55" s="12"/>
-      <c r="E55" s="12"/>
+        <v>64</v>
+      </c>
+      <c r="C55" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="D55" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="E55" t="s" s="11">
+        <v>10</v>
+      </c>
       <c r="F55" s="12"/>
-      <c r="G55" s="12"/>
+      <c r="G55" t="s" s="11">
+        <v>10</v>
+      </c>
     </row>
     <row r="56" ht="21.5" customHeight="1">
       <c r="A56" t="s" s="10">
         <v>8</v>
       </c>
       <c r="B56" t="s" s="11">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C56" t="s" s="11">
         <v>10</v>
@@ -2657,7 +2695,7 @@
         <v>8</v>
       </c>
       <c r="B57" t="s" s="11">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C57" t="s" s="11">
         <v>10</v>
@@ -2678,7 +2716,7 @@
         <v>8</v>
       </c>
       <c r="B58" t="s" s="11">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C58" t="s" s="11">
         <v>10</v>
@@ -2701,7 +2739,7 @@
         <v>8</v>
       </c>
       <c r="B59" t="s" s="11">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C59" t="s" s="11">
         <v>10</v>
@@ -2718,24 +2756,30 @@
       </c>
     </row>
     <row r="60" ht="21.5" customHeight="1">
-      <c r="A60" t="s" s="14">
-        <v>50</v>
+      <c r="A60" t="s" s="10">
+        <v>8</v>
       </c>
       <c r="B60" t="s" s="11">
-        <v>70</v>
-      </c>
-      <c r="C60" s="12"/>
-      <c r="D60" s="12"/>
+        <v>69</v>
+      </c>
+      <c r="C60" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="D60" t="s" s="11">
+        <v>10</v>
+      </c>
       <c r="E60" s="12"/>
       <c r="F60" s="12"/>
-      <c r="G60" s="12"/>
+      <c r="G60" t="s" s="11">
+        <v>10</v>
+      </c>
     </row>
     <row r="61" ht="21.5" customHeight="1">
       <c r="A61" t="s" s="10">
         <v>8</v>
       </c>
       <c r="B61" t="s" s="11">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C61" t="s" s="11">
         <v>10</v>
@@ -2756,7 +2800,7 @@
         <v>8</v>
       </c>
       <c r="B62" t="s" s="11">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C62" t="s" s="11">
         <v>10</v>
@@ -2777,7 +2821,7 @@
         <v>8</v>
       </c>
       <c r="B63" t="s" s="11">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C63" t="s" s="11">
         <v>10</v>
@@ -2796,7 +2840,7 @@
         <v>8</v>
       </c>
       <c r="B64" t="s" s="11">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C64" t="s" s="11">
         <v>10</v>
@@ -2811,24 +2855,32 @@
       </c>
     </row>
     <row r="65" ht="21.5" customHeight="1">
-      <c r="A65" t="s" s="14">
-        <v>50</v>
+      <c r="A65" t="s" s="10">
+        <v>8</v>
       </c>
       <c r="B65" t="s" s="11">
-        <v>75</v>
-      </c>
-      <c r="C65" s="12"/>
-      <c r="D65" s="12"/>
-      <c r="E65" s="12"/>
+        <v>74</v>
+      </c>
+      <c r="C65" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="D65" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="E65" t="s" s="11">
+        <v>10</v>
+      </c>
       <c r="F65" s="12"/>
-      <c r="G65" s="12"/>
+      <c r="G65" t="s" s="11">
+        <v>10</v>
+      </c>
     </row>
     <row r="66" ht="21.5" customHeight="1">
       <c r="A66" t="s" s="10">
         <v>8</v>
       </c>
       <c r="B66" t="s" s="11">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C66" t="s" s="11">
         <v>10</v>
@@ -2845,24 +2897,30 @@
       </c>
     </row>
     <row r="67" ht="21.5" customHeight="1">
-      <c r="A67" t="s" s="14">
-        <v>50</v>
+      <c r="A67" t="s" s="10">
+        <v>8</v>
       </c>
       <c r="B67" t="s" s="11">
-        <v>77</v>
-      </c>
-      <c r="C67" s="12"/>
-      <c r="D67" s="12"/>
+        <v>76</v>
+      </c>
+      <c r="C67" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="D67" t="s" s="11">
+        <v>10</v>
+      </c>
       <c r="E67" s="12"/>
       <c r="F67" s="12"/>
-      <c r="G67" s="12"/>
+      <c r="G67" t="s" s="11">
+        <v>10</v>
+      </c>
     </row>
     <row r="68" ht="21.5" customHeight="1">
       <c r="A68" t="s" s="10">
         <v>8</v>
       </c>
       <c r="B68" t="s" s="11">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C68" t="s" s="11">
         <v>10</v>
@@ -2879,24 +2937,30 @@
       </c>
     </row>
     <row r="69" ht="21.5" customHeight="1">
-      <c r="A69" t="s" s="14">
-        <v>50</v>
+      <c r="A69" t="s" s="10">
+        <v>8</v>
       </c>
       <c r="B69" t="s" s="11">
-        <v>79</v>
-      </c>
-      <c r="C69" s="12"/>
-      <c r="D69" s="12"/>
+        <v>78</v>
+      </c>
+      <c r="C69" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="D69" t="s" s="11">
+        <v>10</v>
+      </c>
       <c r="E69" s="12"/>
       <c r="F69" s="12"/>
-      <c r="G69" s="12"/>
+      <c r="G69" t="s" s="11">
+        <v>10</v>
+      </c>
     </row>
     <row r="70" ht="21.5" customHeight="1">
       <c r="A70" t="s" s="10">
         <v>8</v>
       </c>
       <c r="B70" t="s" s="11">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C70" t="s" s="11">
         <v>10</v>
@@ -2915,7 +2979,7 @@
         <v>8</v>
       </c>
       <c r="B71" t="s" s="11">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C71" t="s" s="11">
         <v>10</v>
@@ -2930,24 +2994,32 @@
       </c>
     </row>
     <row r="72" ht="21.5" customHeight="1">
-      <c r="A72" t="s" s="14">
-        <v>50</v>
+      <c r="A72" t="s" s="10">
+        <v>8</v>
       </c>
       <c r="B72" t="s" s="11">
-        <v>82</v>
-      </c>
-      <c r="C72" s="12"/>
-      <c r="D72" s="12"/>
-      <c r="E72" s="12"/>
+        <v>81</v>
+      </c>
+      <c r="C72" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="D72" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="E72" t="s" s="11">
+        <v>10</v>
+      </c>
       <c r="F72" s="12"/>
-      <c r="G72" s="12"/>
+      <c r="G72" t="s" s="11">
+        <v>10</v>
+      </c>
     </row>
     <row r="73" ht="21.5" customHeight="1">
       <c r="A73" t="s" s="10">
         <v>8</v>
       </c>
       <c r="B73" t="s" s="11">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C73" t="s" s="11">
         <v>10</v>
@@ -2966,7 +3038,7 @@
         <v>8</v>
       </c>
       <c r="B74" t="s" s="11">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C74" t="s" s="11">
         <v>10</v>
@@ -2985,7 +3057,7 @@
         <v>8</v>
       </c>
       <c r="B75" t="s" s="11">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C75" t="s" s="11">
         <v>10</v>
@@ -3002,24 +3074,30 @@
       </c>
     </row>
     <row r="76" ht="21.5" customHeight="1">
-      <c r="A76" t="s" s="14">
-        <v>50</v>
+      <c r="A76" t="s" s="10">
+        <v>8</v>
       </c>
       <c r="B76" t="s" s="11">
-        <v>86</v>
-      </c>
-      <c r="C76" s="12"/>
-      <c r="D76" s="12"/>
+        <v>85</v>
+      </c>
+      <c r="C76" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="D76" t="s" s="11">
+        <v>10</v>
+      </c>
       <c r="E76" s="12"/>
       <c r="F76" s="12"/>
-      <c r="G76" s="12"/>
+      <c r="G76" t="s" s="11">
+        <v>10</v>
+      </c>
     </row>
     <row r="77" ht="21.5" customHeight="1">
       <c r="A77" t="s" s="10">
         <v>8</v>
       </c>
       <c r="B77" t="s" s="11">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C77" t="s" s="11">
         <v>10</v>
@@ -3034,73 +3112,91 @@
       </c>
     </row>
     <row r="78" ht="21.5" customHeight="1">
-      <c r="A78" t="s" s="14">
-        <v>50</v>
+      <c r="A78" t="s" s="10">
+        <v>8</v>
       </c>
       <c r="B78" t="s" s="11">
-        <v>88</v>
-      </c>
-      <c r="C78" s="12"/>
-      <c r="D78" s="12"/>
+        <v>87</v>
+      </c>
+      <c r="C78" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="D78" t="s" s="11">
+        <v>10</v>
+      </c>
       <c r="E78" s="12"/>
       <c r="F78" s="12"/>
-      <c r="G78" s="12"/>
+      <c r="G78" t="s" s="11">
+        <v>10</v>
+      </c>
     </row>
     <row r="79" ht="21.5" customHeight="1">
-      <c r="A79" t="s" s="14">
-        <v>50</v>
+      <c r="A79" t="s" s="10">
+        <v>8</v>
       </c>
       <c r="B79" t="s" s="11">
-        <v>89</v>
-      </c>
-      <c r="C79" s="12"/>
-      <c r="D79" s="12"/>
+        <v>88</v>
+      </c>
+      <c r="C79" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="D79" t="s" s="11">
+        <v>10</v>
+      </c>
       <c r="E79" s="12"/>
       <c r="F79" s="12"/>
-      <c r="G79" s="12"/>
+      <c r="G79" t="s" s="11">
+        <v>10</v>
+      </c>
     </row>
     <row r="80" ht="21.5" customHeight="1">
       <c r="A80" t="s" s="10">
         <v>8</v>
       </c>
       <c r="B80" t="s" s="11">
+        <v>89</v>
+      </c>
+      <c r="C80" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="D80" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="E80" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="F80" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="G80" t="s" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="81" ht="21.5" customHeight="1">
+      <c r="A81" t="s" s="10">
+        <v>8</v>
+      </c>
+      <c r="B81" t="s" s="11">
         <v>90</v>
       </c>
-      <c r="C80" t="s" s="11">
-        <v>10</v>
-      </c>
-      <c r="D80" t="s" s="11">
-        <v>10</v>
-      </c>
-      <c r="E80" t="s" s="11">
-        <v>10</v>
-      </c>
-      <c r="F80" t="s" s="11">
-        <v>10</v>
-      </c>
-      <c r="G80" t="s" s="11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="81" ht="21.5" customHeight="1">
-      <c r="A81" t="s" s="14">
-        <v>50</v>
-      </c>
-      <c r="B81" t="s" s="11">
-        <v>91</v>
-      </c>
-      <c r="C81" s="12"/>
-      <c r="D81" s="12"/>
+      <c r="C81" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="D81" t="s" s="11">
+        <v>10</v>
+      </c>
       <c r="E81" s="12"/>
       <c r="F81" s="12"/>
-      <c r="G81" s="12"/>
+      <c r="G81" t="s" s="11">
+        <v>10</v>
+      </c>
     </row>
     <row r="82" ht="21.5" customHeight="1">
       <c r="A82" t="s" s="10">
         <v>8</v>
       </c>
       <c r="B82" t="s" s="11">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C82" t="s" s="11">
         <v>10</v>
@@ -3123,7 +3219,7 @@
         <v>8</v>
       </c>
       <c r="B83" t="s" s="11">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C83" t="s" s="11">
         <v>10</v>
@@ -3144,7 +3240,7 @@
         <v>8</v>
       </c>
       <c r="B84" t="s" s="11">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C84" t="s" s="11">
         <v>10</v>
@@ -3163,7 +3259,7 @@
         <v>8</v>
       </c>
       <c r="B85" t="s" s="11">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C85" t="s" s="11">
         <v>10</v>
@@ -3178,24 +3274,30 @@
       </c>
     </row>
     <row r="86" ht="21.5" customHeight="1">
-      <c r="A86" t="s" s="14">
-        <v>50</v>
+      <c r="A86" t="s" s="10">
+        <v>8</v>
       </c>
       <c r="B86" t="s" s="11">
-        <v>96</v>
-      </c>
-      <c r="C86" s="12"/>
-      <c r="D86" s="12"/>
+        <v>95</v>
+      </c>
+      <c r="C86" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="D86" t="s" s="11">
+        <v>10</v>
+      </c>
       <c r="E86" s="12"/>
       <c r="F86" s="12"/>
-      <c r="G86" s="12"/>
+      <c r="G86" t="s" s="11">
+        <v>10</v>
+      </c>
     </row>
     <row r="87" ht="21.5" customHeight="1">
       <c r="A87" t="s" s="10">
         <v>8</v>
       </c>
       <c r="B87" t="s" s="11">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C87" t="s" s="11">
         <v>10</v>
@@ -3212,24 +3314,30 @@
       </c>
     </row>
     <row r="88" ht="21.5" customHeight="1">
-      <c r="A88" t="s" s="14">
-        <v>50</v>
+      <c r="A88" t="s" s="10">
+        <v>8</v>
       </c>
       <c r="B88" t="s" s="11">
-        <v>98</v>
-      </c>
-      <c r="C88" s="12"/>
-      <c r="D88" s="12"/>
+        <v>97</v>
+      </c>
+      <c r="C88" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="D88" t="s" s="11">
+        <v>10</v>
+      </c>
       <c r="E88" s="12"/>
       <c r="F88" s="12"/>
-      <c r="G88" s="12"/>
+      <c r="G88" t="s" s="11">
+        <v>10</v>
+      </c>
     </row>
     <row r="89" ht="21.5" customHeight="1">
       <c r="A89" t="s" s="10">
         <v>8</v>
       </c>
       <c r="B89" t="s" s="11">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C89" t="s" s="11">
         <v>10</v>

</xml_diff>